<commit_message>
0307 class roll randomized
</commit_message>
<xml_diff>
--- a/data/quiz0307.xlsx
+++ b/data/quiz0307.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Statistics/R.WD/Class_data/class201601-master/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Statistics/R.WD/Class_data/class201601/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="51720" yWindow="2640" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="319">
   <si>
     <t>과목명 : 생활속의통계학-01(005036)</t>
   </si>
@@ -882,26 +882,162 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Black</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>라</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>마</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>나</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>나</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Black</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -910,160 +1046,33 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>나</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>마</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>나</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Red</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>박강한</t>
+  </si>
+  <si>
+    <t>pkh970211@naver.com</t>
+  </si>
+  <si>
+    <t>010-4265-8848</t>
   </si>
 </sst>
 </file>
@@ -1488,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1601,9 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1631,7 +1642,7 @@
         <v>242</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1702,7 +1713,7 @@
         <v>229</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>255</v>
@@ -1711,7 +1722,7 @@
         <v>242</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1788,10 +1799,10 @@
         <v>231</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1899,10 +1910,10 @@
         <v>41</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>231</v>
@@ -2225,13 +2236,13 @@
         <v>249</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2271,7 +2282,7 @@
         <v>256</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2305,13 +2316,13 @@
         <v>249</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2342,7 +2353,7 @@
         <v>237</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>231</v>
@@ -2351,7 +2362,7 @@
         <v>242</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -2360,38 +2371,30 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3">
-        <v>20141119</v>
+        <v>20162412</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>316</v>
       </c>
       <c r="F23" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>82</v>
+        <v>317</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>302</v>
-      </c>
+      <c r="I23" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="5" t="s">
-        <v>294</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -2400,38 +2403,38 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3">
-        <v>20166231</v>
+        <v>20141119</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>311</v>
+        <v>229</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>231</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>242</v>
+        <v>301</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2440,38 +2443,38 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D25" s="3">
-        <v>20143510</v>
+        <v>20166231</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F25" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>229</v>
+        <v>310</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>315</v>
+        <v>231</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2483,35 +2486,35 @@
         <v>67</v>
       </c>
       <c r="D26" s="3">
-        <v>20153517</v>
+        <v>20143510</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>236</v>
+        <v>313</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>242</v>
+        <v>314</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2520,38 +2523,38 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="3" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D27" s="3">
-        <v>20113124</v>
+        <v>20153517</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F27" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>283</v>
+        <v>235</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>300</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2560,38 +2563,38 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="3" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="D28" s="3">
-        <v>20123829</v>
+        <v>20113124</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F28" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>231</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2600,38 +2603,38 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="3" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="D29" s="3">
-        <v>20132121</v>
+        <v>20123829</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F29" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2640,35 +2643,35 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="D30" s="3">
-        <v>20134227</v>
+        <v>20132121</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F30" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>242</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>250</v>
@@ -2680,38 +2683,38 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="D31" s="3">
-        <v>20163022</v>
+        <v>20134227</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>229</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="L31" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="M31" s="5" t="s">
-        <v>256</v>
-      </c>
       <c r="N31" s="5" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2720,38 +2723,38 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D32" s="3">
-        <v>20121521</v>
+        <v>20163022</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2760,38 +2763,38 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="3" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="D33" s="3">
-        <v>20133827</v>
+        <v>20121521</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F33" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2800,38 +2803,38 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="3" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="D34" s="3">
-        <v>20133914</v>
+        <v>20133827</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F34" s="3">
         <v>4</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>229</v>
+        <v>277</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -2840,38 +2843,38 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="3" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D35" s="3">
-        <v>20156253</v>
+        <v>20133914</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F35" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -2880,35 +2883,35 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="3" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="D36" s="3">
-        <v>20151525</v>
+        <v>20156253</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F36" s="3">
         <v>2</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>250</v>
@@ -2920,29 +2923,39 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="3" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D37" s="3">
-        <v>20154237</v>
+        <v>20151525</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F37" s="3">
         <v>2</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
+        <v>127</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -2950,38 +2963,30 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="3" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="D38" s="3">
-        <v>20151139</v>
+        <v>20154237</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F38" s="3">
         <v>2</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>242</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
       <c r="N38" s="5" t="s">
-        <v>250</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -2990,38 +2995,38 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="3" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D39" s="3">
-        <v>20135233</v>
+        <v>20151139</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F39" s="3">
         <v>2</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3030,38 +3035,38 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="3" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="D40" s="3">
-        <v>20133832</v>
+        <v>20135233</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F40" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -3070,35 +3075,35 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="3" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="D41" s="3">
-        <v>20155423</v>
+        <v>20133832</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F41" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>249</v>
+        <v>278</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="N41" s="5" t="s">
         <v>245</v>
@@ -3110,38 +3115,38 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="3" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="D42" s="3">
-        <v>20163029</v>
+        <v>20155423</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L42" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="M42" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="M42" s="5" t="s">
-        <v>239</v>
-      </c>
       <c r="N42" s="5" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3150,38 +3155,38 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D43" s="3">
-        <v>20156266</v>
+        <v>20163029</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -3190,38 +3195,38 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="3" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D44" s="3">
-        <v>20103932</v>
+        <v>20156266</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F44" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>229</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>242</v>
+        <v>289</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3230,38 +3235,38 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="3" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="D45" s="3">
-        <v>20154244</v>
+        <v>20103932</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F45" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>292</v>
+        <v>229</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -3270,38 +3275,38 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="3" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="D46" s="3">
-        <v>20151528</v>
+        <v>20154244</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F46" s="3">
         <v>2</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -3310,35 +3315,35 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="D47" s="3">
-        <v>20122904</v>
+        <v>20151528</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F47" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="N47" s="5" t="s">
         <v>250</v>
@@ -3350,38 +3355,38 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D48" s="3">
-        <v>20123526</v>
+        <v>20122904</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F48" s="3">
         <v>3</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>231</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -3390,26 +3395,26 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D49" s="3">
-        <v>20156271</v>
+        <v>20123526</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>249</v>
@@ -3430,38 +3435,38 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="3" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="D50" s="3">
-        <v>20163134</v>
+        <v>20156271</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>229</v>
+        <v>295</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>305</v>
+        <v>249</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>307</v>
+        <v>242</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -3470,38 +3475,38 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D51" s="3">
-        <v>20156153</v>
+        <v>20163134</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F51" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>229</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>240</v>
+        <v>304</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>242</v>
+        <v>305</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>242</v>
+        <v>306</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -3510,38 +3515,38 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="3" t="s">
-        <v>84</v>
+        <v>173</v>
       </c>
       <c r="D52" s="3">
-        <v>20156284</v>
+        <v>20156153</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F52" s="3">
         <v>2</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>312</v>
+        <v>229</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>313</v>
+        <v>242</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -3550,38 +3555,38 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="3" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D53" s="3">
-        <v>20154256</v>
+        <v>20156284</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F53" s="3">
         <v>2</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>239</v>
+        <v>311</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>258</v>
+        <v>312</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -3590,38 +3595,38 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="3" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
       <c r="D54" s="3">
-        <v>20112356</v>
+        <v>20154256</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F54" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>250</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -3630,35 +3635,35 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="3" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="D55" s="3">
-        <v>20143155</v>
+        <v>20112356</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F55" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="N55" s="5" t="s">
         <v>250</v>
@@ -3670,38 +3675,38 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="3" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="D56" s="3">
-        <v>20154259</v>
+        <v>20143155</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -3710,38 +3715,38 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="3" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="D57" s="3">
-        <v>20153530</v>
+        <v>20154259</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F57" s="3">
         <v>2</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>242</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>275</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -3750,38 +3755,38 @@
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="3" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="D58" s="3">
-        <v>20154261</v>
+        <v>20153530</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F58" s="3">
         <v>2</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>234</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -3790,118 +3795,118 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="3" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="D59" s="3">
-        <v>20123940</v>
+        <v>20154261</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F59" s="3">
         <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="31" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="3" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="D60" s="3">
-        <v>20135354</v>
+        <v>20123940</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F60" s="3">
         <v>2</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J60" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="N60" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="31" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="3" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="D61" s="3">
-        <v>20142935</v>
+        <v>20135354</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F61" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>236</v>
+        <v>283</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -3910,38 +3915,38 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="3" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="D62" s="3">
-        <v>20156298</v>
+        <v>20142935</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F62" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>292</v>
+        <v>235</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>303</v>
+        <v>236</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>302</v>
+        <v>237</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -3950,38 +3955,38 @@
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="3" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="D63" s="3">
-        <v>20152934</v>
+        <v>20156298</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F63" s="3">
         <v>2</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>239</v>
+        <v>291</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>231</v>
+        <v>301</v>
       </c>
       <c r="M63" s="5" t="s">
         <v>256</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -3990,38 +3995,38 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D64" s="3">
-        <v>20154270</v>
+        <v>20152934</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F64" s="3">
         <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="N64" s="5" t="s">
-        <v>294</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -4030,38 +4035,38 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="3" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="D65" s="3">
-        <v>20132146</v>
+        <v>20154270</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F65" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>249</v>
+        <v>294</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>234</v>
+        <v>293</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -4070,38 +4075,78 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D66" s="3">
-        <v>20123173</v>
+        <v>20132146</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F66" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="N66" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="3">
+        <v>20123173</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F67" s="3">
+        <v>2</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J67" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="L66" s="5" t="s">
+      <c r="K67" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="L67" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="M67" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="N66" s="5" t="s">
-        <v>288</v>
+      <c r="N67" s="5" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>